<commit_message>
Included new line..again... Included support for Pacakge column. Will not prefix arguments with in/out/io if package type is library
</commit_message>
<xml_diff>
--- a/Whiteboarding Template.xlsx
+++ b/Whiteboarding Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James Reames\Documents\UiPath\Development In Progress\WhiteboardToModule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james.reames\Documents\UiPath\GIT\WhiteboardToModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FEA465-260D-4D72-AFC2-35CC099B766D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DD61EC-F1A2-4B2A-A728-8195A249330B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1350" yWindow="2490" windowWidth="1980" windowHeight="1030" xr2:uid="{DED1349C-E413-4137-911C-AD21FE046331}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DED1349C-E413-4137-911C-AD21FE046331}"/>
   </bookViews>
   <sheets>
     <sheet name="Design" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
   <si>
     <t>Workflow</t>
   </si>
@@ -153,6 +153,21 @@
   </si>
   <si>
     <t>&lt;x:Property Name="[[ARGUMENTNAME]]" Type="InOutArgument(x:[[ARGUMENTTYPE]])" /&gt;</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>App_Module2</t>
+  </si>
+  <si>
+    <t>Performer</t>
+  </si>
+  <si>
+    <t>Dispatcher</t>
   </si>
 </sst>
 </file>
@@ -539,22 +554,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02E8452-6399-4051-9869-87D5CD17FA02}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" customWidth="1"/>
-    <col min="2" max="2" width="25.26953125" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" customWidth="1"/>
-    <col min="5" max="5" width="25.453125" customWidth="1"/>
-    <col min="6" max="6" width="18.1796875" customWidth="1"/>
-    <col min="7" max="7" width="23.81640625" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -577,7 +592,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -586,7 +601,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -595,7 +610,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -611,53 +626,56 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A6131D-7D59-449A-938D-D8A42418EB0D}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" customWidth="1"/>
-    <col min="2" max="2" width="25.26953125" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" customWidth="1"/>
-    <col min="5" max="5" width="25.453125" customWidth="1"/>
-    <col min="6" max="6" width="18.1796875" customWidth="1"/>
-    <col min="7" max="7" width="23.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
@@ -665,22 +683,25 @@
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
@@ -688,22 +709,25 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
@@ -711,12 +735,41 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -734,12 +787,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.08984375" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -747,7 +800,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -755,7 +808,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -763,7 +816,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -771,7 +824,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -792,12 +845,12 @@
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -805,7 +858,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -813,7 +866,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -821,7 +874,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -829,7 +882,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -837,7 +890,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -845,7 +898,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -853,7 +906,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -861,7 +914,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -869,7 +922,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>

</xml_diff>